<commit_message>
Ajuste no cadastro de Horários de Jeif
</commit_message>
<xml_diff>
--- a/servidor.xlsx
+++ b/servidor.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -505,6 +505,258 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>236.658.7.88/9</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Célio Vetrano</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>20E</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>01/05/2019</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>{"segunda-feira": "00:00 \u00e0s 00:00", "ter\u00e7a-feira": "00:00 \u00e0s 00:00", "quarta-feira": "00:00 \u00e0s 00:00", "quinta-feira": "00:00 \u00e0s 00:00", "sexta-feira": "00:00 \u00e0s 00:00"}</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>{"segunda-feira": "12:00 \u00e0s 15:00", "ter\u00e7a-feira": "12:00 \u00e0s 15:00", "quarta-feira": "12:00 \u00e0s 15:00", "quinta-feira": "12:00 \u00e0s 15:00", "sexta-feira": "12:00 \u00e0s 15:00"}</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>7E</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Professor de Informática</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>777.777.7.77/7</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Aline Silva</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>15A</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>01/06/2018</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>{"segunda-feira": "00:00 \u00e0s 00:00", "ter\u00e7a-feira": "00:00 \u00e0s 00:00", "quarta-feira": "00:00 \u00e0s 00:00", "quinta-feira": "00:00 \u00e0s 00:00", "sexta-feira": "00:00 \u00e0s 00:00"}</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>{"segunda-feira": "08:00 \u00e0s 12:00", "ter\u00e7a-feira": "08:00 \u00e0s 12:00", "quarta-feira": "08:00 \u00e0s 12:00", "quinta-feira": "08:00 \u00e0s 12:00", "sexta-feira": "08:00 \u00e0s 12:00"}</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>7B</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>professor de educação física</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>666.666.6.66/6</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Alice Burba</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>20E</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>25/06/1985</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>{"segunda-feira": "13:00 \u00e0s 14:00", "ter\u00e7a-feira": "13:00 \u00e0s 14:00", "quarta-feira": "13:00 \u00e0s 14:00", "quinta-feira": "13:00 \u00e0s 14:00", "sexta-feira": "13:00 \u00e0s 14:00"}</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>{"segunda-feira": "08:00 \u00e0s 12:00", "ter\u00e7a-feira": "08:00 \u00e0s 12:00", "quarta-feira": "08:00 \u00e0s 12:00", "quinta-feira": "08:00 \u00e0s 12:00", "sexta-feira": "08:00 \u00e0s 14:00"}</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>6D</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Professor de Educação Infantil</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>555.555.5.55/5</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Tatiana Marques</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>14B</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>01/01/2025</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>{"segunda-feira": "14:00 \u00e0s 15:00", "ter\u00e7a-feira": "14:00 \u00e0s 15:00", "quarta-feira": "14:00 \u00e0s 15:00", "quinta-feira": "14:00 \u00e0s 15:00", "sexta-feira": "14:00 \u00e0s 15:00"}</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>{"segunda-feira": "14:00 \u00e0s 15:00", "ter\u00e7a-feira": "14:00 \u00e0s 15:00", "quarta-feira": "14:00 \u00e0s 15:00", "quinta-feira": "14:00 \u00e0s 15:00", "sexta-feira": "14:00 \u00e0s 15:00"}</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>7A</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>professor</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>333.444.5.66/7</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Marilucia Junqueira</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>20D</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>03/07/1996</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>{"segunda-feira": "00:00 \u00e0s 00:00", "ter\u00e7a-feira": "00:00 \u00e0s 00:00", "quarta-feira": "00:00 \u00e0s 00:00", "quinta-feira": "00:00 \u00e0s 00:00", "sexta-feira": "00:00 \u00e0s 00:00"}</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>{"segunda-feira": "07:00 \u00e0s 11:00", "ter\u00e7a-feira": "07:00 \u00e0s 11:00", "quarta-feira": "07:00 \u00e0s 11:00", "quinta-feira": "07:00 \u00e0s 11:00", "sexta-feira": "07:00 \u00e0s 11:00"}</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>9A</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>professor</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>999.888.7.66/5</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>João Paulo Sarmento</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>22A</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>05/04/1987</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>{"segunda-feira": "09:00 \u00e0s 10:00", "ter\u00e7a-feira": "09:00 \u00e0s 10:00", "quarta-feira": "09:00 \u00e0s 10:00", "quinta-feira": "09:00 \u00e0s 10:00", "sexta-feira": "09:00 \u00e0s 10:00"}</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>{"segunda-feira": "11:00 \u00e0s 15:00", "ter\u00e7a-feira": "10:00 \u00e0s 15:00", "quarta-feira": "10:00 \u00e0s 15:00", "quinta-feira": "10:00 \u00e0s 15:00", "sexta-feira": "10:00 \u00e0s 15:00"}</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>00</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Professor Readaptado</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Gerando o executável da aplicação
</commit_message>
<xml_diff>
--- a/servidor.xlsx
+++ b/servidor.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -550,121 +550,121 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>777.777.7.77/7</t>
+          <t>666.666.6.66/6</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Aline Silva</t>
+          <t>Alice Burba</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>15A</t>
+          <t>20E</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>01/06/2018</t>
+          <t>25/06/1985</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>{"segunda-feira": "00:00 \u00e0s 00:00", "ter\u00e7a-feira": "00:00 \u00e0s 00:00", "quarta-feira": "00:00 \u00e0s 00:00", "quinta-feira": "00:00 \u00e0s 00:00", "sexta-feira": "00:00 \u00e0s 00:00"}</t>
+          <t>{"segunda-feira": "13:00 \u00e0s 14:00", "ter\u00e7a-feira": "13:00 \u00e0s 14:00", "quarta-feira": "13:00 \u00e0s 14:00", "quinta-feira": "13:00 \u00e0s 14:00", "sexta-feira": "13:00 \u00e0s 14:00"}</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>{"segunda-feira": "08:00 \u00e0s 12:00", "ter\u00e7a-feira": "08:00 \u00e0s 12:00", "quarta-feira": "08:00 \u00e0s 12:00", "quinta-feira": "08:00 \u00e0s 12:00", "sexta-feira": "08:00 \u00e0s 12:00"}</t>
+          <t>{"segunda-feira": "08:00 \u00e0s 12:00", "ter\u00e7a-feira": "08:00 \u00e0s 12:00", "quarta-feira": "08:00 \u00e0s 12:00", "quinta-feira": "08:00 \u00e0s 12:00", "sexta-feira": "08:00 \u00e0s 14:00"}</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>7B</t>
+          <t>6D</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>professor de educação física</t>
+          <t>Professor de Educação Infantil</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>666.666.6.66/6</t>
+          <t>555.555.5.55/5</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Alice Burba</t>
+          <t>Tatiana Marques</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>20E</t>
+          <t>14B</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>25/06/1985</t>
+          <t>01/01/2025</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>{"segunda-feira": "13:00 \u00e0s 14:00", "ter\u00e7a-feira": "13:00 \u00e0s 14:00", "quarta-feira": "13:00 \u00e0s 14:00", "quinta-feira": "13:00 \u00e0s 14:00", "sexta-feira": "13:00 \u00e0s 14:00"}</t>
+          <t>{"segunda-feira": "14:00 \u00e0s 15:00", "ter\u00e7a-feira": "14:00 \u00e0s 15:00", "quarta-feira": "14:00 \u00e0s 15:00", "quinta-feira": "14:00 \u00e0s 15:00", "sexta-feira": "14:00 \u00e0s 15:00"}</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>{"segunda-feira": "08:00 \u00e0s 12:00", "ter\u00e7a-feira": "08:00 \u00e0s 12:00", "quarta-feira": "08:00 \u00e0s 12:00", "quinta-feira": "08:00 \u00e0s 12:00", "sexta-feira": "08:00 \u00e0s 14:00"}</t>
+          <t>{"segunda-feira": "14:00 \u00e0s 15:00", "ter\u00e7a-feira": "14:00 \u00e0s 15:00", "quarta-feira": "14:00 \u00e0s 15:00", "quinta-feira": "14:00 \u00e0s 15:00", "sexta-feira": "14:00 \u00e0s 15:00"}</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>6D</t>
+          <t>7A</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Professor de Educação Infantil</t>
+          <t>professor</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>555.555.5.55/5</t>
+          <t>333.444.5.66/7</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Tatiana Marques</t>
+          <t>Marilucia Junqueira</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>14B</t>
+          <t>20D</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>01/01/2025</t>
+          <t>03/07/1996</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>{"segunda-feira": "14:00 \u00e0s 15:00", "ter\u00e7a-feira": "14:00 \u00e0s 15:00", "quarta-feira": "14:00 \u00e0s 15:00", "quinta-feira": "14:00 \u00e0s 15:00", "sexta-feira": "14:00 \u00e0s 15:00"}</t>
+          <t>{"segunda-feira": "00:00 \u00e0s 00:00", "ter\u00e7a-feira": "00:00 \u00e0s 00:00", "quarta-feira": "00:00 \u00e0s 00:00", "quinta-feira": "00:00 \u00e0s 00:00", "sexta-feira": "00:00 \u00e0s 00:00"}</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>{"segunda-feira": "14:00 \u00e0s 15:00", "ter\u00e7a-feira": "14:00 \u00e0s 15:00", "quarta-feira": "14:00 \u00e0s 15:00", "quinta-feira": "14:00 \u00e0s 15:00", "sexta-feira": "14:00 \u00e0s 15:00"}</t>
+          <t>{"segunda-feira": "07:00 \u00e0s 11:00", "ter\u00e7a-feira": "07:00 \u00e0s 11:00", "quarta-feira": "07:00 \u00e0s 11:00", "quinta-feira": "07:00 \u00e0s 11:00", "sexta-feira": "07:00 \u00e0s 11:00"}</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>7A</t>
+          <t>9A</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -676,82 +676,40 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>333.444.5.66/7</t>
+          <t>999.888.7.66/5</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Marilucia Junqueira</t>
+          <t>João Paulo Sarmento</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>20D</t>
+          <t>22A</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>03/07/1996</t>
+          <t>05/04/1987</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>{"segunda-feira": "00:00 \u00e0s 00:00", "ter\u00e7a-feira": "00:00 \u00e0s 00:00", "quarta-feira": "00:00 \u00e0s 00:00", "quinta-feira": "00:00 \u00e0s 00:00", "sexta-feira": "00:00 \u00e0s 00:00"}</t>
+          <t>{"segunda-feira": "09:00 \u00e0s 10:00", "ter\u00e7a-feira": "09:00 \u00e0s 10:00", "quarta-feira": "09:00 \u00e0s 10:00", "quinta-feira": "09:00 \u00e0s 10:00", "sexta-feira": "09:00 \u00e0s 10:00"}</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>{"segunda-feira": "07:00 \u00e0s 11:00", "ter\u00e7a-feira": "07:00 \u00e0s 11:00", "quarta-feira": "07:00 \u00e0s 11:00", "quinta-feira": "07:00 \u00e0s 11:00", "sexta-feira": "07:00 \u00e0s 11:00"}</t>
+          <t>{"segunda-feira": "11:00 \u00e0s 15:00", "ter\u00e7a-feira": "10:00 \u00e0s 15:00", "quarta-feira": "10:00 \u00e0s 15:00", "quinta-feira": "10:00 \u00e0s 15:00", "sexta-feira": "10:00 \u00e0s 15:00"}</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>9A</t>
+          <t>00</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
-        <is>
-          <t>professor</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>999.888.7.66/5</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>João Paulo Sarmento</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>22A</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>05/04/1987</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>{"segunda-feira": "09:00 \u00e0s 10:00", "ter\u00e7a-feira": "09:00 \u00e0s 10:00", "quarta-feira": "09:00 \u00e0s 10:00", "quinta-feira": "09:00 \u00e0s 10:00", "sexta-feira": "09:00 \u00e0s 10:00"}</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>{"segunda-feira": "11:00 \u00e0s 15:00", "ter\u00e7a-feira": "10:00 \u00e0s 15:00", "quarta-feira": "10:00 \u00e0s 15:00", "quinta-feira": "10:00 \u00e0s 15:00", "sexta-feira": "10:00 \u00e0s 15:00"}</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>00</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
         <is>
           <t>Professor Readaptado</t>
         </is>

</xml_diff>